<commit_message>
loaded different household dicts
</commit_message>
<xml_diff>
--- a/data/current_map_data.xlsx
+++ b/data/current_map_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikdrean/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikdrean/Documents/python_projects/map_z_scraper/map_z_scraper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A897408C-7A46-6F49-BEF8-4222A21EC66F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1F34DB-C6EE-C84B-A752-5C3ADAA8F769}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="24620" windowHeight="15020"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="24620" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="compiled_data_1.2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="619">
   <si>
     <t>Location Code</t>
   </si>
@@ -1670,9 +1670,6 @@
     <t>ab2d710fd7ba6935acd84f1d22121335</t>
   </si>
   <si>
-    <t>Antioquia, Bryce &amp; Amy</t>
-  </si>
-  <si>
     <t>4fad8754340f650fc3e78e9fb303e208</t>
   </si>
   <si>
@@ -1811,13 +1808,7 @@
     <t>e68f87e80e4afb7d887fce0dbf8d2404</t>
   </si>
   <si>
-    <t>? Tried to visit once without luck</t>
-  </si>
-  <si>
     <t>485 S 600 E</t>
-  </si>
-  <si>
-    <t>No one lives here. A doctor owns it and will be selling it.</t>
   </si>
   <si>
     <t>e8c1a034593dafc9ee5f3c954636bef8</t>
@@ -1885,11 +1876,17 @@
   <si>
     <t>67bd95d2d532d4b0f05ecfa5c0a3e3b2</t>
   </si>
+  <si>
+    <t xml:space="preserve">? </t>
+  </si>
+  <si>
+    <t>No one lives here. A doctor owns it and will be selling it. Tried to visit once without luck</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2727,14 +2724,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="M223" sqref="M223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -6234,7 +6234,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" ht="368" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>465</v>
       </c>
@@ -7106,9 +7106,6 @@
       <c r="A192" t="s">
         <v>548</v>
       </c>
-      <c r="B192" t="s">
-        <v>549</v>
-      </c>
       <c r="C192" t="s">
         <v>494</v>
       </c>
@@ -7127,13 +7124,13 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B193" t="s">
         <v>500</v>
       </c>
       <c r="C193" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D193" t="s">
         <v>11</v>
@@ -7150,13 +7147,13 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B194" t="s">
         <v>500</v>
       </c>
       <c r="C194" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D194" t="s">
         <v>11</v>
@@ -7173,13 +7170,13 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B195" t="s">
         <v>500</v>
       </c>
       <c r="C195" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D195" t="s">
         <v>11</v>
@@ -7196,13 +7193,13 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B196" t="s">
         <v>500</v>
       </c>
       <c r="C196" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D196" t="s">
         <v>11</v>
@@ -7219,7 +7216,7 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B197" t="s">
         <v>500</v>
@@ -7248,10 +7245,10 @@
         <v>500</v>
       </c>
       <c r="C198" t="s">
+        <v>558</v>
+      </c>
+      <c r="D198" t="s">
         <v>559</v>
-      </c>
-      <c r="D198" t="s">
-        <v>560</v>
       </c>
       <c r="E198" t="s">
         <v>12</v>
@@ -7265,7 +7262,7 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B199" t="s">
         <v>500</v>
@@ -7288,10 +7285,10 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>561</v>
+      </c>
+      <c r="B200" t="s">
         <v>562</v>
-      </c>
-      <c r="B200" t="s">
-        <v>563</v>
       </c>
       <c r="C200" t="s">
         <v>189</v>
@@ -7306,12 +7303,12 @@
         <v>84606</v>
       </c>
       <c r="G200" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B201" t="s">
         <v>500</v>
@@ -7329,7 +7326,7 @@
         <v>84606</v>
       </c>
       <c r="G201" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H201">
         <v>469</v>
@@ -7337,7 +7334,7 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B202" t="s">
         <v>500</v>
@@ -7349,15 +7346,15 @@
         <v>12</v>
       </c>
       <c r="G202" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H202" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B203" t="s">
         <v>500</v>
@@ -7369,7 +7366,7 @@
         <v>12</v>
       </c>
       <c r="G203" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H203">
         <v>541</v>
@@ -7377,7 +7374,7 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B204" t="s">
         <v>500</v>
@@ -7395,15 +7392,15 @@
         <v>84606</v>
       </c>
       <c r="G204" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H204" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B205" t="s">
         <v>500</v>
@@ -7421,12 +7418,12 @@
         <v>84606</v>
       </c>
       <c r="G205" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B206" t="s">
         <v>500</v>
@@ -7444,12 +7441,12 @@
         <v>84606</v>
       </c>
       <c r="G206" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B207" t="s">
         <v>500</v>
@@ -7467,41 +7464,41 @@
         <v>84606</v>
       </c>
       <c r="G207" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H207" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B208" t="s">
         <v>500</v>
       </c>
       <c r="C208" t="s">
+        <v>576</v>
+      </c>
+      <c r="D208" t="s">
+        <v>11</v>
+      </c>
+      <c r="E208" t="s">
+        <v>12</v>
+      </c>
+      <c r="F208">
+        <v>84606</v>
+      </c>
+      <c r="G208" t="s">
+        <v>565</v>
+      </c>
+      <c r="H208" t="s">
         <v>577</v>
-      </c>
-      <c r="D208" t="s">
-        <v>11</v>
-      </c>
-      <c r="E208" t="s">
-        <v>12</v>
-      </c>
-      <c r="F208">
-        <v>84606</v>
-      </c>
-      <c r="G208" t="s">
-        <v>566</v>
-      </c>
-      <c r="H208" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B209" t="s">
         <v>500</v>
@@ -7519,12 +7516,12 @@
         <v>84606</v>
       </c>
       <c r="G209" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B210" t="s">
         <v>500</v>
@@ -7542,15 +7539,15 @@
         <v>84606</v>
       </c>
       <c r="G210" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H210" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B211" t="s">
         <v>500</v>
@@ -7568,15 +7565,15 @@
         <v>84606</v>
       </c>
       <c r="G211" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>582</v>
+      </c>
+      <c r="B212" t="s">
         <v>583</v>
-      </c>
-      <c r="B212" t="s">
-        <v>584</v>
       </c>
       <c r="C212" t="s">
         <v>294</v>
@@ -7591,12 +7588,12 @@
         <v>84606</v>
       </c>
       <c r="G212" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B213" t="s">
         <v>500</v>
@@ -7614,15 +7611,15 @@
         <v>84606</v>
       </c>
       <c r="G213" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H213" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B214" t="s">
         <v>500</v>
@@ -7631,7 +7628,7 @@
         <v>39</v>
       </c>
       <c r="D214" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E214" t="s">
         <v>12</v>
@@ -7640,12 +7637,12 @@
         <v>84102</v>
       </c>
       <c r="G214" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B215" t="s">
         <v>500</v>
@@ -7654,7 +7651,7 @@
         <v>39</v>
       </c>
       <c r="D215" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E215" t="s">
         <v>12</v>
@@ -7663,7 +7660,7 @@
         <v>84102</v>
       </c>
       <c r="G215" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H215">
         <v>445</v>
@@ -7671,7 +7668,7 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B216" t="s">
         <v>500</v>
@@ -7680,7 +7677,7 @@
         <v>39</v>
       </c>
       <c r="D216" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E216" t="s">
         <v>12</v>
@@ -7689,7 +7686,7 @@
         <v>84102</v>
       </c>
       <c r="G216" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H216">
         <v>429</v>
@@ -7697,7 +7694,7 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B217" t="s">
         <v>500</v>
@@ -7715,7 +7712,7 @@
         <v>84606</v>
       </c>
       <c r="G217" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H217">
         <v>626</v>
@@ -7723,13 +7720,13 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B218" t="s">
         <v>500</v>
       </c>
       <c r="C218" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D218" t="s">
         <v>11</v>
@@ -7741,12 +7738,12 @@
         <v>84606</v>
       </c>
       <c r="G218" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B219" t="s">
         <v>500</v>
@@ -7764,19 +7761,19 @@
         <v>84606</v>
       </c>
       <c r="G219" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
+        <v>594</v>
+      </c>
+      <c r="B220" t="s">
+        <v>617</v>
+      </c>
+      <c r="C220" t="s">
         <v>595</v>
       </c>
-      <c r="B220" t="s">
-        <v>596</v>
-      </c>
-      <c r="C220" t="s">
-        <v>597</v>
-      </c>
       <c r="D220" t="s">
         <v>11</v>
       </c>
@@ -7787,21 +7784,21 @@
         <v>84606</v>
       </c>
       <c r="G220" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H220" t="s">
-        <v>598</v>
+        <v>618</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B221" t="s">
         <v>500</v>
       </c>
       <c r="C221" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D221" t="s">
         <v>11</v>
@@ -7813,12 +7810,12 @@
         <v>84606</v>
       </c>
       <c r="G221" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B222" t="s">
         <v>428</v>
@@ -7836,7 +7833,7 @@
         <v>84606</v>
       </c>
       <c r="G222" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.2">
@@ -7859,12 +7856,12 @@
         <v>84606</v>
       </c>
       <c r="G223" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B224" t="s">
         <v>500</v>
@@ -7882,12 +7879,12 @@
         <v>84606</v>
       </c>
       <c r="G224" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B225" t="s">
         <v>500</v>
@@ -7905,12 +7902,12 @@
         <v>84606</v>
       </c>
       <c r="G225" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B226" t="s">
         <v>500</v>
@@ -7928,96 +7925,96 @@
         <v>84606</v>
       </c>
       <c r="G226" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H226" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B227" t="s">
         <v>500</v>
       </c>
       <c r="G227" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
+        <v>603</v>
+      </c>
+      <c r="B228" t="s">
+        <v>604</v>
+      </c>
+      <c r="G228" t="s">
+        <v>565</v>
+      </c>
+      <c r="H228" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
         <v>606</v>
-      </c>
-      <c r="B228" t="s">
-        <v>607</v>
-      </c>
-      <c r="G228" t="s">
-        <v>566</v>
-      </c>
-      <c r="H228" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A229" t="s">
-        <v>609</v>
       </c>
       <c r="B229" t="s">
         <v>500</v>
       </c>
       <c r="G229" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B230" t="s">
         <v>500</v>
       </c>
       <c r="G230" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H230" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B231" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="G231" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H231" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B232" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="G232" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H232" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="G233" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
in middle of fixing change, add, delete hh
</commit_message>
<xml_diff>
--- a/data/current_map_data.xlsx
+++ b/data/current_map_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikdrean/Documents/python_projects/map_z_scraper/map_z_scraper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1F34DB-C6EE-C84B-A752-5C3ADAA8F769}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE8A07-C2A0-1E4C-AD08-775D8245A5E5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="24620" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="440" windowWidth="24620" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="compiled_data_1.2" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>c76377cdc9f943d43c5ae80a43bf80e2</t>
   </si>
   <si>
-    <t>Allen, Drake &amp; Kaylee</t>
-  </si>
-  <si>
     <t>441 S 500 E</t>
   </si>
   <si>
@@ -631,9 +628,6 @@
     <t>b8debbf9d1b6ad38dc2647183d147a81</t>
   </si>
   <si>
-    <t>Guti√©rrez, Aurelio &amp; Paula</t>
-  </si>
-  <si>
     <t>650 E 500 S Apt 3</t>
   </si>
   <si>
@@ -1282,9 +1276,6 @@
     <t>25be8ca0e436924c75ab30b12b3410af</t>
   </si>
   <si>
-    <t>Scofield, Jeffrey David &amp; Mar√≠ Angeles</t>
-  </si>
-  <si>
     <t>333 S 400 E</t>
   </si>
   <si>
@@ -1400,9 +1391,6 @@
   </si>
   <si>
     <t>Wall, Cody Lane</t>
-  </si>
-  <si>
-    <t>562 E 400 S</t>
   </si>
   <si>
     <t>He works at Taco Paraiso on 300 s. She works at Vivint. She works on Sundays. They speak English and are open. Katherine's brother lives with them. He says, "I am not active, but I have my reasons."</t>
@@ -1881,6 +1869,18 @@
   </si>
   <si>
     <t>No one lives here. A doctor owns it and will be selling it. Tried to visit once without luck</t>
+  </si>
+  <si>
+    <t>Allen, Drake &amp; Kaylee Arlene</t>
+  </si>
+  <si>
+    <t>Gutiérrez, Aurelio &amp; Paula</t>
+  </si>
+  <si>
+    <t>Scofield, Jeffrey David &amp; Marí Angeles</t>
+  </si>
+  <si>
+    <t>562 East 400 South</t>
   </si>
 </sst>
 </file>
@@ -2727,8 +2727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="M223" sqref="M223"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2816,10 +2816,10 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -2836,13 +2836,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -2859,13 +2859,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -2882,13 +2882,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -2905,13 +2905,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -2925,13 +2925,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -2948,13 +2948,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -2968,13 +2968,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -2991,13 +2991,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -3014,13 +3014,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -3037,13 +3037,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>50</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -3060,13 +3060,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -3083,13 +3083,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" t="s">
-        <v>57</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -3106,13 +3106,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>59</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -3129,13 +3129,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -3152,13 +3152,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>66</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -3175,13 +3175,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
         <v>67</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -3198,13 +3198,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -3221,13 +3221,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>73</v>
-      </c>
-      <c r="C22" t="s">
-        <v>74</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -3244,13 +3244,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
         <v>75</v>
       </c>
-      <c r="B23" t="s">
-        <v>76</v>
-      </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -3267,13 +3267,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
         <v>77</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>78</v>
-      </c>
-      <c r="C24" t="s">
-        <v>79</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -3290,13 +3290,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
         <v>80</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>81</v>
-      </c>
-      <c r="C25" t="s">
-        <v>82</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -3313,13 +3313,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
         <v>83</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>84</v>
-      </c>
-      <c r="C26" t="s">
-        <v>85</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -3336,13 +3336,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" t="s">
         <v>86</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>87</v>
-      </c>
-      <c r="C27" t="s">
-        <v>88</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -3359,13 +3359,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
         <v>89</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>90</v>
-      </c>
-      <c r="C28" t="s">
-        <v>91</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -3379,13 +3379,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="s">
         <v>92</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>93</v>
-      </c>
-      <c r="C29" t="s">
-        <v>94</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -3402,13 +3402,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" t="s">
         <v>95</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>96</v>
-      </c>
-      <c r="C30" t="s">
-        <v>97</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -3425,13 +3425,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
         <v>98</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>99</v>
-      </c>
-      <c r="C31" t="s">
-        <v>100</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -3448,13 +3448,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
         <v>101</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>102</v>
-      </c>
-      <c r="C32" t="s">
-        <v>103</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -3468,13 +3468,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
         <v>104</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>105</v>
-      </c>
-      <c r="C33" t="s">
-        <v>106</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -3491,13 +3491,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
         <v>107</v>
       </c>
-      <c r="B34" t="s">
-        <v>108</v>
-      </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -3514,13 +3514,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s">
         <v>109</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>110</v>
-      </c>
-      <c r="C35" t="s">
-        <v>111</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -3537,13 +3537,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" t="s">
         <v>112</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>113</v>
-      </c>
-      <c r="C36" t="s">
-        <v>114</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -3560,13 +3560,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
         <v>115</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>116</v>
-      </c>
-      <c r="C37" t="s">
-        <v>117</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -3583,13 +3583,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" t="s">
         <v>118</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>119</v>
-      </c>
-      <c r="C38" t="s">
-        <v>120</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -3606,13 +3606,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" t="s">
         <v>121</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>122</v>
-      </c>
-      <c r="C39" t="s">
-        <v>123</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -3629,13 +3629,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" t="s">
         <v>124</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>125</v>
-      </c>
-      <c r="C40" t="s">
-        <v>126</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -3652,13 +3652,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" t="s">
         <v>127</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>128</v>
-      </c>
-      <c r="C41" t="s">
-        <v>129</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -3675,13 +3675,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" t="s">
         <v>130</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>131</v>
-      </c>
-      <c r="C42" t="s">
-        <v>132</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -3698,39 +3698,39 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" t="s">
         <v>133</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>134</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <v>84606</v>
+      </c>
+      <c r="G43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" t="s">
         <v>135</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43">
-        <v>84606</v>
-      </c>
-      <c r="G43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" t="s">
         <v>137</v>
       </c>
-      <c r="B44" t="s">
-        <v>138</v>
-      </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -3747,13 +3747,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" t="s">
         <v>139</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>140</v>
-      </c>
-      <c r="C45" t="s">
-        <v>141</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -3770,13 +3770,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" t="s">
         <v>142</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>143</v>
-      </c>
-      <c r="C46" t="s">
-        <v>144</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -3793,13 +3793,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" t="s">
         <v>145</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>146</v>
-      </c>
-      <c r="C47" t="s">
-        <v>147</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -3813,39 +3813,39 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" t="s">
         <v>148</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>149</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48">
+        <v>84606</v>
+      </c>
+      <c r="G48" t="s">
         <v>150</v>
       </c>
-      <c r="D48" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48">
-        <v>84606</v>
-      </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>151</v>
-      </c>
-      <c r="H48" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" t="s">
         <v>153</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>154</v>
-      </c>
-      <c r="C49" t="s">
-        <v>155</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -3862,13 +3862,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" t="s">
         <v>156</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>157</v>
-      </c>
-      <c r="C50" t="s">
-        <v>158</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
@@ -3885,13 +3885,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" t="s">
         <v>159</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>160</v>
-      </c>
-      <c r="C51" t="s">
-        <v>161</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
@@ -3908,13 +3908,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>161</v>
+      </c>
+      <c r="B52" t="s">
         <v>162</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>163</v>
-      </c>
-      <c r="C52" t="s">
-        <v>164</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
@@ -3928,13 +3928,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" t="s">
         <v>165</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>166</v>
-      </c>
-      <c r="C53" t="s">
-        <v>167</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
@@ -3951,13 +3951,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" t="s">
         <v>168</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>169</v>
-      </c>
-      <c r="C54" t="s">
-        <v>170</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -3974,13 +3974,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" t="s">
         <v>171</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>172</v>
-      </c>
-      <c r="C55" t="s">
-        <v>173</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -3997,13 +3997,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" t="s">
         <v>174</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>175</v>
-      </c>
-      <c r="C56" t="s">
-        <v>176</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -4020,13 +4020,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" t="s">
         <v>177</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>178</v>
-      </c>
-      <c r="C57" t="s">
-        <v>179</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
@@ -4043,13 +4043,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" t="s">
         <v>180</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>181</v>
-      </c>
-      <c r="C58" t="s">
-        <v>182</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
@@ -4066,13 +4066,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>182</v>
+      </c>
+      <c r="B59" t="s">
         <v>183</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>184</v>
-      </c>
-      <c r="C59" t="s">
-        <v>185</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -4089,13 +4089,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B60" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C60" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -4112,13 +4112,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61" t="s">
         <v>187</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>188</v>
-      </c>
-      <c r="C61" t="s">
-        <v>189</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -4135,13 +4135,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>189</v>
+      </c>
+      <c r="B62" t="s">
         <v>190</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>191</v>
-      </c>
-      <c r="C62" t="s">
-        <v>192</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -4158,13 +4158,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>192</v>
+      </c>
+      <c r="B63" t="s">
         <v>193</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>194</v>
-      </c>
-      <c r="C63" t="s">
-        <v>195</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
@@ -4181,13 +4181,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" t="s">
         <v>196</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>197</v>
-      </c>
-      <c r="C64" t="s">
-        <v>198</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -4204,13 +4204,13 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>198</v>
+      </c>
+      <c r="B65" t="s">
         <v>199</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>200</v>
-      </c>
-      <c r="C65" t="s">
-        <v>201</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>
@@ -4221,13 +4221,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>201</v>
+      </c>
+      <c r="B66" t="s">
+        <v>616</v>
+      </c>
+      <c r="C66" t="s">
         <v>202</v>
-      </c>
-      <c r="B66" t="s">
-        <v>203</v>
-      </c>
-      <c r="C66" t="s">
-        <v>204</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
@@ -4244,13 +4244,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>203</v>
+      </c>
+      <c r="B67" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" t="s">
         <v>205</v>
-      </c>
-      <c r="B67" t="s">
-        <v>206</v>
-      </c>
-      <c r="C67" t="s">
-        <v>207</v>
       </c>
       <c r="D67" t="s">
         <v>11</v>
@@ -4267,13 +4267,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" t="s">
         <v>208</v>
-      </c>
-      <c r="B68" t="s">
-        <v>209</v>
-      </c>
-      <c r="C68" t="s">
-        <v>210</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -4290,13 +4290,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>209</v>
+      </c>
+      <c r="B69" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" t="s">
         <v>211</v>
-      </c>
-      <c r="B69" t="s">
-        <v>212</v>
-      </c>
-      <c r="C69" t="s">
-        <v>213</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -4313,13 +4313,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" t="s">
         <v>214</v>
-      </c>
-      <c r="B70" t="s">
-        <v>215</v>
-      </c>
-      <c r="C70" t="s">
-        <v>216</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
@@ -4336,13 +4336,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>215</v>
+      </c>
+      <c r="B71" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71" t="s">
         <v>217</v>
-      </c>
-      <c r="B71" t="s">
-        <v>218</v>
-      </c>
-      <c r="C71" t="s">
-        <v>219</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -4359,13 +4359,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" t="s">
+        <v>219</v>
+      </c>
+      <c r="C72" t="s">
         <v>220</v>
-      </c>
-      <c r="B72" t="s">
-        <v>221</v>
-      </c>
-      <c r="C72" t="s">
-        <v>222</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
@@ -4382,13 +4382,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>221</v>
+      </c>
+      <c r="B73" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" t="s">
         <v>223</v>
-      </c>
-      <c r="B73" t="s">
-        <v>224</v>
-      </c>
-      <c r="C73" t="s">
-        <v>225</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
@@ -4405,39 +4405,39 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" t="s">
         <v>226</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74">
+        <v>84606</v>
+      </c>
+      <c r="G74" t="s">
+        <v>150</v>
+      </c>
+      <c r="H74" t="s">
         <v>227</v>
-      </c>
-      <c r="C74" t="s">
-        <v>228</v>
-      </c>
-      <c r="D74" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" t="s">
-        <v>12</v>
-      </c>
-      <c r="F74">
-        <v>84606</v>
-      </c>
-      <c r="G74" t="s">
-        <v>151</v>
-      </c>
-      <c r="H74" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>228</v>
+      </c>
+      <c r="B75" t="s">
+        <v>229</v>
+      </c>
+      <c r="C75" t="s">
         <v>230</v>
-      </c>
-      <c r="B75" t="s">
-        <v>231</v>
-      </c>
-      <c r="C75" t="s">
-        <v>232</v>
       </c>
       <c r="D75" t="s">
         <v>11</v>
@@ -4454,13 +4454,13 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>231</v>
+      </c>
+      <c r="B76" t="s">
+        <v>232</v>
+      </c>
+      <c r="C76" t="s">
         <v>233</v>
-      </c>
-      <c r="B76" t="s">
-        <v>234</v>
-      </c>
-      <c r="C76" t="s">
-        <v>235</v>
       </c>
       <c r="D76" t="s">
         <v>11</v>
@@ -4477,13 +4477,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>234</v>
+      </c>
+      <c r="B77" t="s">
+        <v>235</v>
+      </c>
+      <c r="C77" t="s">
         <v>236</v>
-      </c>
-      <c r="B77" t="s">
-        <v>237</v>
-      </c>
-      <c r="C77" t="s">
-        <v>238</v>
       </c>
       <c r="D77" t="s">
         <v>11</v>
@@ -4500,13 +4500,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>237</v>
+      </c>
+      <c r="B78" t="s">
+        <v>238</v>
+      </c>
+      <c r="C78" t="s">
         <v>239</v>
-      </c>
-      <c r="B78" t="s">
-        <v>240</v>
-      </c>
-      <c r="C78" t="s">
-        <v>241</v>
       </c>
       <c r="D78" t="s">
         <v>11</v>
@@ -4523,13 +4523,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>240</v>
+      </c>
+      <c r="B79" t="s">
+        <v>241</v>
+      </c>
+      <c r="C79" t="s">
         <v>242</v>
-      </c>
-      <c r="B79" t="s">
-        <v>243</v>
-      </c>
-      <c r="C79" t="s">
-        <v>244</v>
       </c>
       <c r="D79" t="s">
         <v>11</v>
@@ -4546,13 +4546,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>243</v>
+      </c>
+      <c r="B80" t="s">
+        <v>244</v>
+      </c>
+      <c r="C80" t="s">
         <v>245</v>
-      </c>
-      <c r="B80" t="s">
-        <v>246</v>
-      </c>
-      <c r="C80" t="s">
-        <v>247</v>
       </c>
       <c r="D80" t="s">
         <v>11</v>
@@ -4569,13 +4569,13 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>246</v>
+      </c>
+      <c r="B81" t="s">
+        <v>247</v>
+      </c>
+      <c r="C81" t="s">
         <v>248</v>
-      </c>
-      <c r="B81" t="s">
-        <v>249</v>
-      </c>
-      <c r="C81" t="s">
-        <v>250</v>
       </c>
       <c r="D81" t="s">
         <v>11</v>
@@ -4592,13 +4592,13 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>249</v>
+      </c>
+      <c r="B82" t="s">
+        <v>250</v>
+      </c>
+      <c r="C82" t="s">
         <v>251</v>
-      </c>
-      <c r="B82" t="s">
-        <v>252</v>
-      </c>
-      <c r="C82" t="s">
-        <v>253</v>
       </c>
       <c r="D82" t="s">
         <v>11</v>
@@ -4615,14 +4615,14 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>252</v>
+      </c>
+      <c r="B83" t="s">
+        <v>253</v>
+      </c>
+      <c r="C83" t="s">
         <v>254</v>
       </c>
-      <c r="B83" t="s">
-        <v>255</v>
-      </c>
-      <c r="C83" t="s">
-        <v>256</v>
-      </c>
       <c r="D83" t="s">
         <v>11</v>
       </c>
@@ -4630,18 +4630,18 @@
         <v>12</v>
       </c>
       <c r="G83" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>255</v>
+      </c>
+      <c r="B84" t="s">
+        <v>256</v>
+      </c>
+      <c r="C84" t="s">
         <v>257</v>
-      </c>
-      <c r="B84" t="s">
-        <v>258</v>
-      </c>
-      <c r="C84" t="s">
-        <v>259</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
@@ -4658,13 +4658,13 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>258</v>
+      </c>
+      <c r="B85" t="s">
+        <v>259</v>
+      </c>
+      <c r="C85" t="s">
         <v>260</v>
-      </c>
-      <c r="B85" t="s">
-        <v>261</v>
-      </c>
-      <c r="C85" t="s">
-        <v>262</v>
       </c>
       <c r="D85" t="s">
         <v>11</v>
@@ -4681,13 +4681,13 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>261</v>
+      </c>
+      <c r="B86" t="s">
+        <v>262</v>
+      </c>
+      <c r="C86" t="s">
         <v>263</v>
-      </c>
-      <c r="B86" t="s">
-        <v>264</v>
-      </c>
-      <c r="C86" t="s">
-        <v>265</v>
       </c>
       <c r="D86" t="s">
         <v>11</v>
@@ -4704,13 +4704,13 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>264</v>
+      </c>
+      <c r="B87" t="s">
+        <v>265</v>
+      </c>
+      <c r="C87" t="s">
         <v>266</v>
-      </c>
-      <c r="B87" t="s">
-        <v>267</v>
-      </c>
-      <c r="C87" t="s">
-        <v>268</v>
       </c>
       <c r="D87" t="s">
         <v>11</v>
@@ -4727,13 +4727,13 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>267</v>
+      </c>
+      <c r="B88" t="s">
+        <v>268</v>
+      </c>
+      <c r="C88" t="s">
         <v>269</v>
-      </c>
-      <c r="B88" t="s">
-        <v>270</v>
-      </c>
-      <c r="C88" t="s">
-        <v>271</v>
       </c>
       <c r="D88" t="s">
         <v>11</v>
@@ -4750,13 +4750,13 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>270</v>
+      </c>
+      <c r="B89" t="s">
+        <v>271</v>
+      </c>
+      <c r="C89" t="s">
         <v>272</v>
-      </c>
-      <c r="B89" t="s">
-        <v>273</v>
-      </c>
-      <c r="C89" t="s">
-        <v>274</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
@@ -4773,13 +4773,13 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>273</v>
+      </c>
+      <c r="B90" t="s">
+        <v>274</v>
+      </c>
+      <c r="C90" t="s">
         <v>275</v>
-      </c>
-      <c r="B90" t="s">
-        <v>276</v>
-      </c>
-      <c r="C90" t="s">
-        <v>277</v>
       </c>
       <c r="D90" t="s">
         <v>11</v>
@@ -4790,13 +4790,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>276</v>
+      </c>
+      <c r="B91" t="s">
+        <v>277</v>
+      </c>
+      <c r="C91" t="s">
         <v>278</v>
-      </c>
-      <c r="B91" t="s">
-        <v>279</v>
-      </c>
-      <c r="C91" t="s">
-        <v>280</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
@@ -4813,13 +4813,13 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>279</v>
+      </c>
+      <c r="B92" t="s">
+        <v>280</v>
+      </c>
+      <c r="C92" t="s">
         <v>281</v>
-      </c>
-      <c r="B92" t="s">
-        <v>282</v>
-      </c>
-      <c r="C92" t="s">
-        <v>283</v>
       </c>
       <c r="D92" t="s">
         <v>11</v>
@@ -4836,13 +4836,13 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B93" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C93" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
@@ -4856,13 +4856,13 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>284</v>
+      </c>
+      <c r="B94" t="s">
+        <v>285</v>
+      </c>
+      <c r="C94" t="s">
         <v>286</v>
-      </c>
-      <c r="B94" t="s">
-        <v>287</v>
-      </c>
-      <c r="C94" t="s">
-        <v>288</v>
       </c>
       <c r="D94" t="s">
         <v>11</v>
@@ -4879,13 +4879,13 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>287</v>
+      </c>
+      <c r="B95" t="s">
+        <v>288</v>
+      </c>
+      <c r="C95" t="s">
         <v>289</v>
-      </c>
-      <c r="B95" t="s">
-        <v>290</v>
-      </c>
-      <c r="C95" t="s">
-        <v>291</v>
       </c>
       <c r="D95" t="s">
         <v>11</v>
@@ -4902,13 +4902,13 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>290</v>
+      </c>
+      <c r="B96" t="s">
+        <v>291</v>
+      </c>
+      <c r="C96" t="s">
         <v>292</v>
-      </c>
-      <c r="B96" t="s">
-        <v>293</v>
-      </c>
-      <c r="C96" t="s">
-        <v>294</v>
       </c>
       <c r="D96" t="s">
         <v>11</v>
@@ -4925,13 +4925,13 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>293</v>
+      </c>
+      <c r="B97" t="s">
+        <v>294</v>
+      </c>
+      <c r="C97" t="s">
         <v>295</v>
-      </c>
-      <c r="B97" t="s">
-        <v>296</v>
-      </c>
-      <c r="C97" t="s">
-        <v>297</v>
       </c>
       <c r="D97" t="s">
         <v>11</v>
@@ -4942,13 +4942,13 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>296</v>
+      </c>
+      <c r="B98" t="s">
+        <v>297</v>
+      </c>
+      <c r="C98" t="s">
         <v>298</v>
-      </c>
-      <c r="B98" t="s">
-        <v>299</v>
-      </c>
-      <c r="C98" t="s">
-        <v>300</v>
       </c>
       <c r="D98" t="s">
         <v>11</v>
@@ -4965,13 +4965,13 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B99" t="s">
+        <v>300</v>
+      </c>
+      <c r="C99" t="s">
         <v>301</v>
-      </c>
-      <c r="B99" t="s">
-        <v>302</v>
-      </c>
-      <c r="C99" t="s">
-        <v>303</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
@@ -4988,13 +4988,13 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>302</v>
+      </c>
+      <c r="B100" t="s">
+        <v>303</v>
+      </c>
+      <c r="C100" t="s">
         <v>304</v>
-      </c>
-      <c r="B100" t="s">
-        <v>305</v>
-      </c>
-      <c r="C100" t="s">
-        <v>306</v>
       </c>
       <c r="D100" t="s">
         <v>11</v>
@@ -5011,39 +5011,39 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>305</v>
+      </c>
+      <c r="B101" t="s">
+        <v>306</v>
+      </c>
+      <c r="C101" t="s">
         <v>307</v>
       </c>
-      <c r="B101" t="s">
+      <c r="D101" t="s">
+        <v>11</v>
+      </c>
+      <c r="E101" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101">
+        <v>84606</v>
+      </c>
+      <c r="G101" t="s">
+        <v>150</v>
+      </c>
+      <c r="H101" t="s">
         <v>308</v>
-      </c>
-      <c r="C101" t="s">
-        <v>309</v>
-      </c>
-      <c r="D101" t="s">
-        <v>11</v>
-      </c>
-      <c r="E101" t="s">
-        <v>12</v>
-      </c>
-      <c r="F101">
-        <v>84606</v>
-      </c>
-      <c r="G101" t="s">
-        <v>151</v>
-      </c>
-      <c r="H101" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>309</v>
+      </c>
+      <c r="B102" t="s">
+        <v>310</v>
+      </c>
+      <c r="C102" t="s">
         <v>311</v>
-      </c>
-      <c r="B102" t="s">
-        <v>312</v>
-      </c>
-      <c r="C102" t="s">
-        <v>313</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
@@ -5060,13 +5060,13 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>312</v>
+      </c>
+      <c r="B103" t="s">
+        <v>313</v>
+      </c>
+      <c r="C103" t="s">
         <v>314</v>
-      </c>
-      <c r="B103" t="s">
-        <v>315</v>
-      </c>
-      <c r="C103" t="s">
-        <v>316</v>
       </c>
       <c r="D103" t="s">
         <v>11</v>
@@ -5083,13 +5083,13 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>315</v>
+      </c>
+      <c r="B104" t="s">
+        <v>316</v>
+      </c>
+      <c r="C104" t="s">
         <v>317</v>
-      </c>
-      <c r="B104" t="s">
-        <v>318</v>
-      </c>
-      <c r="C104" t="s">
-        <v>319</v>
       </c>
       <c r="D104" t="s">
         <v>11</v>
@@ -5106,13 +5106,13 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>318</v>
+      </c>
+      <c r="B105" t="s">
+        <v>319</v>
+      </c>
+      <c r="C105" t="s">
         <v>320</v>
-      </c>
-      <c r="B105" t="s">
-        <v>321</v>
-      </c>
-      <c r="C105" t="s">
-        <v>322</v>
       </c>
       <c r="D105" t="s">
         <v>11</v>
@@ -5129,13 +5129,13 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B106" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C106" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D106" t="s">
         <v>11</v>
@@ -5152,13 +5152,13 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>323</v>
+      </c>
+      <c r="B107" t="s">
+        <v>324</v>
+      </c>
+      <c r="C107" t="s">
         <v>325</v>
-      </c>
-      <c r="B107" t="s">
-        <v>326</v>
-      </c>
-      <c r="C107" t="s">
-        <v>327</v>
       </c>
       <c r="D107" t="s">
         <v>11</v>
@@ -5175,39 +5175,39 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>326</v>
+      </c>
+      <c r="B108" t="s">
+        <v>327</v>
+      </c>
+      <c r="C108" t="s">
         <v>328</v>
       </c>
-      <c r="B108" t="s">
+      <c r="D108" t="s">
+        <v>11</v>
+      </c>
+      <c r="E108" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108">
+        <v>84606</v>
+      </c>
+      <c r="G108" t="s">
+        <v>150</v>
+      </c>
+      <c r="H108" t="s">
         <v>329</v>
-      </c>
-      <c r="C108" t="s">
-        <v>330</v>
-      </c>
-      <c r="D108" t="s">
-        <v>11</v>
-      </c>
-      <c r="E108" t="s">
-        <v>12</v>
-      </c>
-      <c r="F108">
-        <v>84606</v>
-      </c>
-      <c r="G108" t="s">
-        <v>151</v>
-      </c>
-      <c r="H108" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>330</v>
+      </c>
+      <c r="B109" t="s">
+        <v>331</v>
+      </c>
+      <c r="C109" t="s">
         <v>332</v>
-      </c>
-      <c r="B109" t="s">
-        <v>333</v>
-      </c>
-      <c r="C109" t="s">
-        <v>334</v>
       </c>
       <c r="D109" t="s">
         <v>11</v>
@@ -5221,13 +5221,13 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>333</v>
+      </c>
+      <c r="B110" t="s">
+        <v>334</v>
+      </c>
+      <c r="C110" t="s">
         <v>335</v>
-      </c>
-      <c r="B110" t="s">
-        <v>336</v>
-      </c>
-      <c r="C110" t="s">
-        <v>337</v>
       </c>
       <c r="D110" t="s">
         <v>11</v>
@@ -5244,13 +5244,13 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>336</v>
+      </c>
+      <c r="B111" t="s">
+        <v>337</v>
+      </c>
+      <c r="C111" t="s">
         <v>338</v>
-      </c>
-      <c r="B111" t="s">
-        <v>339</v>
-      </c>
-      <c r="C111" t="s">
-        <v>340</v>
       </c>
       <c r="D111" t="s">
         <v>11</v>
@@ -5267,13 +5267,13 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>339</v>
+      </c>
+      <c r="B112" t="s">
+        <v>340</v>
+      </c>
+      <c r="C112" t="s">
         <v>341</v>
-      </c>
-      <c r="B112" t="s">
-        <v>342</v>
-      </c>
-      <c r="C112" t="s">
-        <v>343</v>
       </c>
       <c r="D112" t="s">
         <v>11</v>
@@ -5290,13 +5290,13 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>342</v>
+      </c>
+      <c r="B113" t="s">
+        <v>343</v>
+      </c>
+      <c r="C113" t="s">
         <v>344</v>
-      </c>
-      <c r="B113" t="s">
-        <v>345</v>
-      </c>
-      <c r="C113" t="s">
-        <v>346</v>
       </c>
       <c r="D113" t="s">
         <v>11</v>
@@ -5313,13 +5313,13 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>345</v>
+      </c>
+      <c r="B114" t="s">
+        <v>346</v>
+      </c>
+      <c r="C114" t="s">
         <v>347</v>
-      </c>
-      <c r="B114" t="s">
-        <v>348</v>
-      </c>
-      <c r="C114" t="s">
-        <v>349</v>
       </c>
       <c r="D114" t="s">
         <v>11</v>
@@ -5336,13 +5336,13 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>348</v>
+      </c>
+      <c r="B115" t="s">
+        <v>349</v>
+      </c>
+      <c r="C115" t="s">
         <v>350</v>
-      </c>
-      <c r="B115" t="s">
-        <v>351</v>
-      </c>
-      <c r="C115" t="s">
-        <v>352</v>
       </c>
       <c r="D115" t="s">
         <v>11</v>
@@ -5359,13 +5359,13 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>351</v>
+      </c>
+      <c r="B116" t="s">
+        <v>352</v>
+      </c>
+      <c r="C116" t="s">
         <v>353</v>
-      </c>
-      <c r="B116" t="s">
-        <v>354</v>
-      </c>
-      <c r="C116" t="s">
-        <v>355</v>
       </c>
       <c r="D116" t="s">
         <v>11</v>
@@ -5382,13 +5382,13 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>354</v>
+      </c>
+      <c r="B117" t="s">
+        <v>355</v>
+      </c>
+      <c r="C117" t="s">
         <v>356</v>
-      </c>
-      <c r="B117" t="s">
-        <v>357</v>
-      </c>
-      <c r="C117" t="s">
-        <v>358</v>
       </c>
       <c r="D117" t="s">
         <v>11</v>
@@ -5405,13 +5405,13 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B118" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C118" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D118" t="s">
         <v>11</v>
@@ -5428,13 +5428,13 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>359</v>
+      </c>
+      <c r="B119" t="s">
+        <v>360</v>
+      </c>
+      <c r="C119" t="s">
         <v>361</v>
-      </c>
-      <c r="B119" t="s">
-        <v>362</v>
-      </c>
-      <c r="C119" t="s">
-        <v>363</v>
       </c>
       <c r="D119" t="s">
         <v>11</v>
@@ -5448,13 +5448,13 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>362</v>
+      </c>
+      <c r="B120" t="s">
+        <v>363</v>
+      </c>
+      <c r="C120" t="s">
         <v>364</v>
-      </c>
-      <c r="B120" t="s">
-        <v>365</v>
-      </c>
-      <c r="C120" t="s">
-        <v>366</v>
       </c>
       <c r="D120" t="s">
         <v>11</v>
@@ -5468,13 +5468,13 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>365</v>
+      </c>
+      <c r="B121" t="s">
+        <v>366</v>
+      </c>
+      <c r="C121" t="s">
         <v>367</v>
-      </c>
-      <c r="B121" t="s">
-        <v>368</v>
-      </c>
-      <c r="C121" t="s">
-        <v>369</v>
       </c>
       <c r="D121" t="s">
         <v>11</v>
@@ -5491,13 +5491,13 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>368</v>
+      </c>
+      <c r="B122" t="s">
+        <v>369</v>
+      </c>
+      <c r="C122" t="s">
         <v>370</v>
-      </c>
-      <c r="B122" t="s">
-        <v>371</v>
-      </c>
-      <c r="C122" t="s">
-        <v>372</v>
       </c>
       <c r="D122" t="s">
         <v>11</v>
@@ -5514,13 +5514,13 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>371</v>
+      </c>
+      <c r="B123" t="s">
+        <v>372</v>
+      </c>
+      <c r="C123" t="s">
         <v>373</v>
-      </c>
-      <c r="B123" t="s">
-        <v>374</v>
-      </c>
-      <c r="C123" t="s">
-        <v>375</v>
       </c>
       <c r="D123" t="s">
         <v>11</v>
@@ -5537,13 +5537,13 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B124" t="s">
+        <v>375</v>
+      </c>
+      <c r="C124" t="s">
         <v>376</v>
-      </c>
-      <c r="B124" t="s">
-        <v>377</v>
-      </c>
-      <c r="C124" t="s">
-        <v>378</v>
       </c>
       <c r="D124" t="s">
         <v>11</v>
@@ -5560,13 +5560,13 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>377</v>
+      </c>
+      <c r="B125" t="s">
+        <v>378</v>
+      </c>
+      <c r="C125" t="s">
         <v>379</v>
-      </c>
-      <c r="B125" t="s">
-        <v>380</v>
-      </c>
-      <c r="C125" t="s">
-        <v>381</v>
       </c>
       <c r="D125" t="s">
         <v>11</v>
@@ -5583,13 +5583,13 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B126" t="s">
+        <v>381</v>
+      </c>
+      <c r="C126" t="s">
         <v>382</v>
-      </c>
-      <c r="B126" t="s">
-        <v>383</v>
-      </c>
-      <c r="C126" t="s">
-        <v>384</v>
       </c>
       <c r="D126" t="s">
         <v>11</v>
@@ -5606,13 +5606,13 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>383</v>
+      </c>
+      <c r="B127" t="s">
+        <v>384</v>
+      </c>
+      <c r="C127" t="s">
         <v>385</v>
-      </c>
-      <c r="B127" t="s">
-        <v>386</v>
-      </c>
-      <c r="C127" t="s">
-        <v>387</v>
       </c>
       <c r="D127" t="s">
         <v>11</v>
@@ -5629,13 +5629,13 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>386</v>
+      </c>
+      <c r="B128" t="s">
+        <v>387</v>
+      </c>
+      <c r="C128" t="s">
         <v>388</v>
-      </c>
-      <c r="B128" t="s">
-        <v>389</v>
-      </c>
-      <c r="C128" t="s">
-        <v>390</v>
       </c>
       <c r="D128" t="s">
         <v>11</v>
@@ -5652,13 +5652,13 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>389</v>
+      </c>
+      <c r="B129" t="s">
+        <v>390</v>
+      </c>
+      <c r="C129" t="s">
         <v>391</v>
-      </c>
-      <c r="B129" t="s">
-        <v>392</v>
-      </c>
-      <c r="C129" t="s">
-        <v>393</v>
       </c>
       <c r="D129" t="s">
         <v>11</v>
@@ -5675,13 +5675,13 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>392</v>
+      </c>
+      <c r="B130" t="s">
+        <v>393</v>
+      </c>
+      <c r="C130" t="s">
         <v>394</v>
-      </c>
-      <c r="B130" t="s">
-        <v>395</v>
-      </c>
-      <c r="C130" t="s">
-        <v>396</v>
       </c>
       <c r="D130" t="s">
         <v>11</v>
@@ -5698,13 +5698,13 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>395</v>
+      </c>
+      <c r="B131" t="s">
+        <v>396</v>
+      </c>
+      <c r="C131" t="s">
         <v>397</v>
-      </c>
-      <c r="B131" t="s">
-        <v>398</v>
-      </c>
-      <c r="C131" t="s">
-        <v>399</v>
       </c>
       <c r="D131" t="s">
         <v>11</v>
@@ -5721,13 +5721,13 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B132" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C132" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D132" t="s">
         <v>11</v>
@@ -5744,39 +5744,39 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B133" t="s">
+        <v>400</v>
+      </c>
+      <c r="C133" t="s">
+        <v>401</v>
+      </c>
+      <c r="D133" t="s">
+        <v>11</v>
+      </c>
+      <c r="E133" t="s">
+        <v>12</v>
+      </c>
+      <c r="F133">
+        <v>84606</v>
+      </c>
+      <c r="G133" t="s">
+        <v>150</v>
+      </c>
+      <c r="H133" t="s">
         <v>402</v>
-      </c>
-      <c r="C133" t="s">
-        <v>403</v>
-      </c>
-      <c r="D133" t="s">
-        <v>11</v>
-      </c>
-      <c r="E133" t="s">
-        <v>12</v>
-      </c>
-      <c r="F133">
-        <v>84606</v>
-      </c>
-      <c r="G133" t="s">
-        <v>151</v>
-      </c>
-      <c r="H133" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>403</v>
+      </c>
+      <c r="B134" t="s">
+        <v>404</v>
+      </c>
+      <c r="C134" t="s">
         <v>405</v>
-      </c>
-      <c r="B134" t="s">
-        <v>406</v>
-      </c>
-      <c r="C134" t="s">
-        <v>407</v>
       </c>
       <c r="D134" t="s">
         <v>11</v>
@@ -5793,13 +5793,13 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>406</v>
+      </c>
+      <c r="B135" t="s">
+        <v>407</v>
+      </c>
+      <c r="C135" t="s">
         <v>408</v>
-      </c>
-      <c r="B135" t="s">
-        <v>409</v>
-      </c>
-      <c r="C135" t="s">
-        <v>410</v>
       </c>
       <c r="D135" t="s">
         <v>11</v>
@@ -5816,13 +5816,13 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>409</v>
+      </c>
+      <c r="B136" t="s">
+        <v>410</v>
+      </c>
+      <c r="C136" t="s">
         <v>411</v>
-      </c>
-      <c r="B136" t="s">
-        <v>412</v>
-      </c>
-      <c r="C136" t="s">
-        <v>413</v>
       </c>
       <c r="D136" t="s">
         <v>11</v>
@@ -5839,13 +5839,13 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>412</v>
+      </c>
+      <c r="B137" t="s">
+        <v>413</v>
+      </c>
+      <c r="C137" t="s">
         <v>414</v>
-      </c>
-      <c r="B137" t="s">
-        <v>415</v>
-      </c>
-      <c r="C137" t="s">
-        <v>416</v>
       </c>
       <c r="D137" t="s">
         <v>11</v>
@@ -5862,13 +5862,13 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B138" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C138" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D138" t="s">
         <v>11</v>
@@ -5885,13 +5885,13 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B139" t="s">
-        <v>420</v>
+        <v>617</v>
       </c>
       <c r="C139" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D139" t="s">
         <v>11</v>
@@ -5908,13 +5908,13 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B140" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C140" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D140" t="s">
         <v>11</v>
@@ -5931,13 +5931,13 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B141" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C141" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D141" t="s">
         <v>11</v>
@@ -5954,13 +5954,13 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B142" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C142" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D142" t="s">
         <v>11</v>
@@ -5977,13 +5977,13 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B143" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C143" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D143" t="s">
         <v>11</v>
@@ -6000,13 +6000,13 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B144" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C144" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D144" t="s">
         <v>11</v>
@@ -6023,13 +6023,13 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B145" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C145" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D145" t="s">
         <v>11</v>
@@ -6046,39 +6046,39 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>436</v>
+      </c>
+      <c r="B146" t="s">
+        <v>437</v>
+      </c>
+      <c r="C146" t="s">
+        <v>438</v>
+      </c>
+      <c r="D146" t="s">
+        <v>11</v>
+      </c>
+      <c r="E146" t="s">
+        <v>12</v>
+      </c>
+      <c r="F146">
+        <v>84606</v>
+      </c>
+      <c r="G146" t="s">
+        <v>150</v>
+      </c>
+      <c r="H146" t="s">
         <v>439</v>
-      </c>
-      <c r="B146" t="s">
-        <v>440</v>
-      </c>
-      <c r="C146" t="s">
-        <v>441</v>
-      </c>
-      <c r="D146" t="s">
-        <v>11</v>
-      </c>
-      <c r="E146" t="s">
-        <v>12</v>
-      </c>
-      <c r="F146">
-        <v>84606</v>
-      </c>
-      <c r="G146" t="s">
-        <v>151</v>
-      </c>
-      <c r="H146" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B147" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C147" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D147" t="s">
         <v>11</v>
@@ -6095,13 +6095,13 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B148" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C148" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D148" t="s">
         <v>11</v>
@@ -6118,13 +6118,13 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B149" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C149" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D149" t="s">
         <v>11</v>
@@ -6141,13 +6141,13 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B150" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C150" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D150" t="s">
         <v>11</v>
@@ -6164,13 +6164,13 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B151" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C151" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D151" t="s">
         <v>11</v>
@@ -6187,13 +6187,13 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B152" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C152" t="s">
-        <v>460</v>
+        <v>618</v>
       </c>
       <c r="D152" t="s">
         <v>11</v>
@@ -6208,18 +6208,18 @@
         <v>18</v>
       </c>
       <c r="H152" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B153" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C153" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D153" t="s">
         <v>11</v>
@@ -6236,13 +6236,13 @@
     </row>
     <row r="154" spans="1:8" ht="368" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B154" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C154" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D154" t="s">
         <v>11</v>
@@ -6254,21 +6254,21 @@
         <v>84606</v>
       </c>
       <c r="G154" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B155" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C155" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D155" t="s">
         <v>11</v>
@@ -6285,13 +6285,13 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B156" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C156" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D156" t="s">
         <v>11</v>
@@ -6308,13 +6308,13 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B157" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C157" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D157" t="s">
         <v>11</v>
@@ -6331,13 +6331,13 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B158" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C158" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D158" t="s">
         <v>11</v>
@@ -6354,13 +6354,13 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B159" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C159" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D159" t="s">
         <v>11</v>
@@ -6377,13 +6377,13 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B160" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C160" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D160" t="s">
         <v>11</v>
@@ -6400,13 +6400,13 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B161" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C161" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D161" t="s">
         <v>11</v>
@@ -6423,13 +6423,13 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B162" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C162" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D162" t="s">
         <v>11</v>
@@ -6444,18 +6444,18 @@
         <v>13</v>
       </c>
       <c r="H162" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B163" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C163" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D163" t="s">
         <v>11</v>
@@ -6472,27 +6472,27 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B164" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G164" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="H164" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B165" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C165" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D165" t="s">
         <v>11</v>
@@ -6501,19 +6501,19 @@
         <v>12</v>
       </c>
       <c r="G165" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B166" t="s">
+        <v>496</v>
+      </c>
+      <c r="C166" t="s">
         <v>500</v>
       </c>
-      <c r="C166" t="s">
-        <v>504</v>
-      </c>
       <c r="D166" t="s">
         <v>11</v>
       </c>
@@ -6524,18 +6524,18 @@
         <v>84606</v>
       </c>
       <c r="G166" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B167" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C167" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D167" t="s">
         <v>11</v>
@@ -6547,18 +6547,18 @@
         <v>84606</v>
       </c>
       <c r="G167" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B168" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C168" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D168" t="s">
         <v>11</v>
@@ -6570,18 +6570,18 @@
         <v>84606</v>
       </c>
       <c r="G168" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B169" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C169" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D169" t="s">
         <v>11</v>
@@ -6593,18 +6593,18 @@
         <v>84606</v>
       </c>
       <c r="G169" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B170" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C170" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D170" t="s">
         <v>11</v>
@@ -6616,18 +6616,18 @@
         <v>84606</v>
       </c>
       <c r="G170" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B171" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C171" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D171" t="s">
         <v>11</v>
@@ -6639,18 +6639,18 @@
         <v>84606</v>
       </c>
       <c r="G171" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B172" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C172" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D172" t="s">
         <v>11</v>
@@ -6662,18 +6662,18 @@
         <v>84606</v>
       </c>
       <c r="G172" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B173" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C173" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D173" t="s">
         <v>11</v>
@@ -6685,18 +6685,18 @@
         <v>84606</v>
       </c>
       <c r="G173" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B174" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C174" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D174" t="s">
         <v>11</v>
@@ -6708,18 +6708,18 @@
         <v>84606</v>
       </c>
       <c r="G174" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B175" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C175" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D175" t="s">
         <v>11</v>
@@ -6731,18 +6731,18 @@
         <v>84606</v>
       </c>
       <c r="G175" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B176" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C176" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D176" t="s">
         <v>11</v>
@@ -6754,18 +6754,18 @@
         <v>84606</v>
       </c>
       <c r="G176" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B177" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C177" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D177" t="s">
         <v>11</v>
@@ -6777,18 +6777,18 @@
         <v>84606</v>
       </c>
       <c r="G177" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B178" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C178" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D178" t="s">
         <v>11</v>
@@ -6800,18 +6800,18 @@
         <v>84606</v>
       </c>
       <c r="G178" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B179" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C179" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D179" t="s">
         <v>11</v>
@@ -6823,18 +6823,18 @@
         <v>84606</v>
       </c>
       <c r="G179" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="B180" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C180" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D180" t="s">
         <v>11</v>
@@ -6846,18 +6846,18 @@
         <v>84606</v>
       </c>
       <c r="G180" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B181" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C181" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D181" t="s">
         <v>11</v>
@@ -6869,18 +6869,18 @@
         <v>84606</v>
       </c>
       <c r="G181" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B182" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C182" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D182" t="s">
         <v>11</v>
@@ -6892,18 +6892,18 @@
         <v>84606</v>
       </c>
       <c r="G182" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B183" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C183" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D183" t="s">
         <v>11</v>
@@ -6915,18 +6915,18 @@
         <v>84606</v>
       </c>
       <c r="G183" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B184" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C184" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D184" t="s">
         <v>11</v>
@@ -6938,18 +6938,18 @@
         <v>84606</v>
       </c>
       <c r="G184" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B185" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C185" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D185" t="s">
         <v>11</v>
@@ -6961,18 +6961,18 @@
         <v>84606</v>
       </c>
       <c r="G185" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B186" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C186" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D186" t="s">
         <v>11</v>
@@ -6984,18 +6984,18 @@
         <v>84606</v>
       </c>
       <c r="G186" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B187" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C187" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D187" t="s">
         <v>11</v>
@@ -7007,18 +7007,18 @@
         <v>84606</v>
       </c>
       <c r="G187" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B188" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C188" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D188" t="s">
         <v>11</v>
@@ -7030,18 +7030,18 @@
         <v>84606</v>
       </c>
       <c r="G188" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B189" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C189" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="D189" t="s">
         <v>11</v>
@@ -7053,18 +7053,18 @@
         <v>84606</v>
       </c>
       <c r="G189" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B190" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C190" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D190" t="s">
         <v>11</v>
@@ -7076,18 +7076,18 @@
         <v>84606</v>
       </c>
       <c r="G190" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B191" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C191" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D191" t="s">
         <v>11</v>
@@ -7099,15 +7099,15 @@
         <v>84606</v>
       </c>
       <c r="G191" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C192" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D192" t="s">
         <v>11</v>
@@ -7119,18 +7119,18 @@
         <v>84606</v>
       </c>
       <c r="G192" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B193" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C193" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D193" t="s">
         <v>11</v>
@@ -7142,18 +7142,18 @@
         <v>84606</v>
       </c>
       <c r="G193" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B194" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C194" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="D194" t="s">
         <v>11</v>
@@ -7165,18 +7165,18 @@
         <v>84606</v>
       </c>
       <c r="G194" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B195" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C195" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D195" t="s">
         <v>11</v>
@@ -7188,18 +7188,18 @@
         <v>84606</v>
       </c>
       <c r="G195" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B196" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C196" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="D196" t="s">
         <v>11</v>
@@ -7211,18 +7211,18 @@
         <v>84606</v>
       </c>
       <c r="G196" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B197" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C197" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D197" t="s">
         <v>11</v>
@@ -7234,21 +7234,21 @@
         <v>84606</v>
       </c>
       <c r="G197" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B198" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C198" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D198" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="E198" t="s">
         <v>12</v>
@@ -7257,18 +7257,18 @@
         <v>84663</v>
       </c>
       <c r="G198" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B199" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C199" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D199" t="s">
         <v>11</v>
@@ -7280,18 +7280,18 @@
         <v>84606</v>
       </c>
       <c r="G199" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B200" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C200" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D200" t="s">
         <v>11</v>
@@ -7303,18 +7303,18 @@
         <v>84606</v>
       </c>
       <c r="G200" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B201" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C201" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D201" t="s">
         <v>11</v>
@@ -7326,7 +7326,7 @@
         <v>84606</v>
       </c>
       <c r="G201" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H201">
         <v>469</v>
@@ -7334,10 +7334,10 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B202" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D202" t="s">
         <v>11</v>
@@ -7346,18 +7346,18 @@
         <v>12</v>
       </c>
       <c r="G202" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H202" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B203" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D203" t="s">
         <v>11</v>
@@ -7366,7 +7366,7 @@
         <v>12</v>
       </c>
       <c r="G203" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H203">
         <v>541</v>
@@ -7374,13 +7374,13 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B204" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C204" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D204" t="s">
         <v>11</v>
@@ -7392,21 +7392,21 @@
         <v>84606</v>
       </c>
       <c r="G204" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H204" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B205" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C205" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D205" t="s">
         <v>11</v>
@@ -7418,18 +7418,18 @@
         <v>84606</v>
       </c>
       <c r="G205" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B206" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C206" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D206" t="s">
         <v>11</v>
@@ -7441,15 +7441,15 @@
         <v>84606</v>
       </c>
       <c r="G206" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B207" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C207" t="s">
         <v>17</v>
@@ -7464,21 +7464,21 @@
         <v>84606</v>
       </c>
       <c r="G207" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H207" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B208" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C208" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="D208" t="s">
         <v>11</v>
@@ -7490,21 +7490,21 @@
         <v>84606</v>
       </c>
       <c r="G208" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H208" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B209" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C209" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D209" t="s">
         <v>11</v>
@@ -7516,18 +7516,18 @@
         <v>84606</v>
       </c>
       <c r="G209" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B210" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C210" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D210" t="s">
         <v>11</v>
@@ -7539,21 +7539,21 @@
         <v>84606</v>
       </c>
       <c r="G210" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H210" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B211" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C211" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D211" t="s">
         <v>11</v>
@@ -7565,18 +7565,18 @@
         <v>84606</v>
       </c>
       <c r="G211" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="B212" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C212" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D212" t="s">
         <v>11</v>
@@ -7588,18 +7588,18 @@
         <v>84606</v>
       </c>
       <c r="G212" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B213" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C213" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D213" t="s">
         <v>11</v>
@@ -7611,24 +7611,24 @@
         <v>84606</v>
       </c>
       <c r="G213" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H213" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B214" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C214" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D214" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E214" t="s">
         <v>12</v>
@@ -7637,21 +7637,21 @@
         <v>84102</v>
       </c>
       <c r="G214" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B215" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C215" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D215" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E215" t="s">
         <v>12</v>
@@ -7660,7 +7660,7 @@
         <v>84102</v>
       </c>
       <c r="G215" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H215">
         <v>445</v>
@@ -7668,16 +7668,16 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B216" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C216" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D216" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E216" t="s">
         <v>12</v>
@@ -7686,7 +7686,7 @@
         <v>84102</v>
       </c>
       <c r="G216" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H216">
         <v>429</v>
@@ -7694,13 +7694,13 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="B217" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C217" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D217" t="s">
         <v>11</v>
@@ -7712,7 +7712,7 @@
         <v>84606</v>
       </c>
       <c r="G217" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H217">
         <v>626</v>
@@ -7720,13 +7720,13 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B218" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C218" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="D218" t="s">
         <v>11</v>
@@ -7738,18 +7738,18 @@
         <v>84606</v>
       </c>
       <c r="G218" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B219" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C219" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D219" t="s">
         <v>11</v>
@@ -7761,18 +7761,18 @@
         <v>84606</v>
       </c>
       <c r="G219" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="B220" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C220" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D220" t="s">
         <v>11</v>
@@ -7784,21 +7784,21 @@
         <v>84606</v>
       </c>
       <c r="G220" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H220" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B221" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C221" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D221" t="s">
         <v>11</v>
@@ -7810,18 +7810,18 @@
         <v>84606</v>
       </c>
       <c r="G221" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B222" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C222" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D222" t="s">
         <v>11</v>
@@ -7833,18 +7833,18 @@
         <v>84606</v>
       </c>
       <c r="G222" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B223" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C223" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D223" t="s">
         <v>11</v>
@@ -7856,18 +7856,18 @@
         <v>84606</v>
       </c>
       <c r="G223" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B224" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C224" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D224" t="s">
         <v>11</v>
@@ -7879,18 +7879,18 @@
         <v>84606</v>
       </c>
       <c r="G224" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B225" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C225" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D225" t="s">
         <v>11</v>
@@ -7902,18 +7902,18 @@
         <v>84606</v>
       </c>
       <c r="G225" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B226" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C226" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D226" t="s">
         <v>11</v>
@@ -7925,96 +7925,96 @@
         <v>84606</v>
       </c>
       <c r="G226" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H226" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B227" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G227" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B228" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="G228" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H228" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="B229" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G229" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B230" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G230" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H230" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B231" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="G231" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H231" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B232" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="G232" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="H232" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="G233" t="s">
         <v>13</v>

</xml_diff>